<commit_message>
Oppgave 1, 2 og 3 fungerer optimalt
</commit_message>
<xml_diff>
--- a/kgdata.xlsx
+++ b/kgdata.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:F1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,6 +460,62 @@
       <c r="F1" s="1" t="inlineStr">
         <is>
           <t>foresatt_pnr</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Solveig Imsdal</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Bekkeveien 100</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>91997087</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>09079233221</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Ole Nordmann</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Alvestien 39</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>91997087</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>09079089332</t>
         </is>
       </c>
     </row>
@@ -474,7 +530,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,25 +541,20 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>index</t>
+          <t>barnehage_id</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>barnehage_id</t>
+          <t>barnehage_navn</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>barnehage_navn</t>
+          <t>barnehage_antall_plasser</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>barnehage_antall_plasser</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>barnehage_ledige_plasser</t>
         </is>
@@ -514,20 +565,17 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="inlineStr">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>Sunshine Preschool</t>
         </is>
       </c>
+      <c r="D2" t="n">
+        <v>50</v>
+      </c>
       <c r="E2" t="n">
-        <v>50</v>
-      </c>
-      <c r="F2" t="n">
         <v>13</v>
       </c>
     </row>
@@ -536,20 +584,17 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="n">
         <v>2</v>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>Happy Days Nursery</t>
         </is>
       </c>
+      <c r="D3" t="n">
+        <v>25</v>
+      </c>
       <c r="E3" t="n">
-        <v>25</v>
-      </c>
-      <c r="F3" t="n">
         <v>2</v>
       </c>
     </row>
@@ -558,20 +603,17 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" t="n">
         <v>3</v>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>123 Learning Center</t>
         </is>
       </c>
+      <c r="D4" t="n">
+        <v>35</v>
+      </c>
       <c r="E4" t="n">
-        <v>35</v>
-      </c>
-      <c r="F4" t="n">
         <v>4</v>
       </c>
     </row>
@@ -580,20 +622,17 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C5" t="n">
         <v>4</v>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>ABC Kindergarten</t>
         </is>
       </c>
+      <c r="D5" t="n">
+        <v>12</v>
+      </c>
       <c r="E5" t="n">
-        <v>12</v>
-      </c>
-      <c r="F5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -602,20 +641,17 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>4</v>
-      </c>
-      <c r="C6" t="n">
         <v>5</v>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>Tiny Tots Academy</t>
         </is>
       </c>
+      <c r="D6" t="n">
+        <v>15</v>
+      </c>
       <c r="E6" t="n">
-        <v>15</v>
-      </c>
-      <c r="F6" t="n">
         <v>5</v>
       </c>
     </row>
@@ -624,20 +660,17 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>5</v>
-      </c>
-      <c r="C7" t="n">
         <v>6</v>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>Giggles and Grins Childcare</t>
         </is>
       </c>
+      <c r="D7" t="n">
+        <v>10</v>
+      </c>
       <c r="E7" t="n">
-        <v>10</v>
-      </c>
-      <c r="F7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -646,20 +679,17 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>6</v>
-      </c>
-      <c r="C8" t="n">
         <v>7</v>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>Playful Pals Daycare</t>
         </is>
       </c>
+      <c r="D8" t="n">
+        <v>40</v>
+      </c>
       <c r="E8" t="n">
-        <v>40</v>
-      </c>
-      <c r="F8" t="n">
         <v>6</v>
       </c>
     </row>
@@ -674,7 +704,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -691,6 +721,19 @@
       <c r="C1" s="1" t="inlineStr">
         <is>
           <t>barn_pnr</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>09012356472</t>
         </is>
       </c>
     </row>
@@ -705,7 +748,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -785,10 +828,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
         <v>2</v>
@@ -806,8 +849,16 @@
         </is>
       </c>
       <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>2020-12-09</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>1100000</t>
+        </is>
+      </c>
       <c r="N2" t="inlineStr">
         <is>
           <t>Ja</t>
@@ -819,10 +870,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
         <v>2</v>
@@ -830,18 +881,44 @@
       <c r="E3" t="n">
         <v>1</v>
       </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>hei</t>
+        </is>
+      </c>
       <c r="J3" t="inlineStr">
         <is>
           <t>Sunshine Preschool</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>2025-05-07</t>
+        </is>
+      </c>
+      <c r="M3" t="n">
+        <v>1100000</v>
+      </c>
       <c r="N3" t="inlineStr">
         <is>
           <t>Ja</t>
@@ -853,10 +930,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
         <v>2</v>
@@ -864,19 +941,101 @@
       <c r="E4" t="n">
         <v>1</v>
       </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>hei</t>
+        </is>
+      </c>
       <c r="J4" t="inlineStr">
         <is>
           <t>Sunshine Preschool</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>2025-05-07</t>
+        </is>
+      </c>
+      <c r="M4" t="n">
+        <v>1100000</v>
+      </c>
       <c r="N4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>hei</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Sunshine Preschool</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>2025-05-07</t>
+        </is>
+      </c>
+      <c r="M5" t="n">
+        <v>1100000</v>
+      </c>
+      <c r="N5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>